<commit_message>
updated outputs, added precision_recall_t.py
</commit_message>
<xml_diff>
--- a/outputs/fft-o__Oscillospirales.xlsx
+++ b/outputs/fft-o__Oscillospirales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanxinli/Desktop/project/BlindKameris-new/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B391DD8-BDB0-3748-BE03-AD7C68E8A1C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681B156A-E495-1B4E-B891-4DC5B1371222}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="600" windowWidth="28800" windowHeight="15880" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="g__Ruminococcus_E-LSVM" sheetId="1" r:id="rId1"/>
@@ -27,18 +27,17 @@
     <sheet name="f__CAG-382-b" sheetId="12" r:id="rId12"/>
     <sheet name="f__Ruminococcaceae-b" sheetId="13" r:id="rId13"/>
     <sheet name="g__Ruminococcus_E-t" sheetId="14" r:id="rId14"/>
-    <sheet name="f__Lachnospiracea-t" sheetId="15" r:id="rId15"/>
+    <sheet name="f__Lachnospiraceae-t" sheetId="15" r:id="rId15"/>
     <sheet name="g__Prevotella-t" sheetId="16" r:id="rId16"/>
     <sheet name="g__C941-t" sheetId="17" r:id="rId17"/>
     <sheet name="g__RC9-t" sheetId="18" r:id="rId18"/>
-    <sheet name="g__CAG-791-t" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2788" uniqueCount="704">
   <si>
     <t>f__Acutalibacteraceae</t>
   </si>
@@ -22154,1106 +22153,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:J34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2">
-        <v>0.6528129269188242</v>
-      </c>
-      <c r="C2">
-        <v>4.0924313269491332E-4</v>
-      </c>
-      <c r="D2">
-        <v>1.687834880472206E-4</v>
-      </c>
-      <c r="E2">
-        <v>6.0941466850486937E-5</v>
-      </c>
-      <c r="F2">
-        <v>3.9460408600952091E-4</v>
-      </c>
-      <c r="G2">
-        <v>0.34615350090757391</v>
-      </c>
-      <c r="H2">
-        <v>0.6528129269188242</v>
-      </c>
-      <c r="I2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3">
-        <v>0.50865742842359996</v>
-      </c>
-      <c r="C3">
-        <v>1.285802888176385E-2</v>
-      </c>
-      <c r="D3">
-        <v>1.2083239339197219E-4</v>
-      </c>
-      <c r="E3">
-        <v>1.2788108164152771E-2</v>
-      </c>
-      <c r="F3">
-        <v>2.889850959820443E-3</v>
-      </c>
-      <c r="G3">
-        <v>0.46268575117727101</v>
-      </c>
-      <c r="H3">
-        <v>0.50865742842359996</v>
-      </c>
-      <c r="I3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4">
-        <v>0.82446459983033848</v>
-      </c>
-      <c r="C4">
-        <v>1.059155427032378E-3</v>
-      </c>
-      <c r="D4">
-        <v>2.460825532482701E-3</v>
-      </c>
-      <c r="E4">
-        <v>1.0882273439018571E-3</v>
-      </c>
-      <c r="F4">
-        <v>1.5290540731895061E-3</v>
-      </c>
-      <c r="G4">
-        <v>0.16939813779305499</v>
-      </c>
-      <c r="H4">
-        <v>0.82446459983033848</v>
-      </c>
-      <c r="I4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5">
-        <v>0.24028204329191119</v>
-      </c>
-      <c r="C5">
-        <v>1.8164888452018489E-5</v>
-      </c>
-      <c r="D5">
-        <v>8.3306389255857656E-3</v>
-      </c>
-      <c r="E5">
-        <v>5.5281309962742315E-4</v>
-      </c>
-      <c r="F5">
-        <v>5.1152503711675533E-2</v>
-      </c>
-      <c r="G5">
-        <v>0.69966383608274807</v>
-      </c>
-      <c r="H5">
-        <v>0.69966383608274807</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6">
-        <v>0.14769335007214901</v>
-      </c>
-      <c r="C6">
-        <v>1.4659766542851349E-5</v>
-      </c>
-      <c r="D6">
-        <v>8.7770194255638642E-5</v>
-      </c>
-      <c r="E6">
-        <v>1.8219094749791369E-4</v>
-      </c>
-      <c r="F6">
-        <v>7.7944114299593049E-5</v>
-      </c>
-      <c r="G6">
-        <v>0.85194408490525508</v>
-      </c>
-      <c r="H6">
-        <v>0.85194408490525508</v>
-      </c>
-      <c r="I6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7">
-        <v>0.59825161875392963</v>
-      </c>
-      <c r="C7">
-        <v>1.2935533909483659E-2</v>
-      </c>
-      <c r="D7">
-        <v>3.9565690296555087E-2</v>
-      </c>
-      <c r="E7">
-        <v>7.7284880856323072E-4</v>
-      </c>
-      <c r="F7">
-        <v>4.897614588742085E-4</v>
-      </c>
-      <c r="G7">
-        <v>0.34798454677259399</v>
-      </c>
-      <c r="H7">
-        <v>0.59825161875392963</v>
-      </c>
-      <c r="I7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8">
-        <v>0.45949403569805941</v>
-      </c>
-      <c r="C8">
-        <v>3.9502120547768643E-3</v>
-      </c>
-      <c r="D8">
-        <v>7.5739003832259552E-2</v>
-      </c>
-      <c r="E8">
-        <v>9.4810211610756121E-4</v>
-      </c>
-      <c r="F8">
-        <v>3.5558773652050498E-6</v>
-      </c>
-      <c r="G8">
-        <v>0.45986509042143148</v>
-      </c>
-      <c r="H8">
-        <v>0.45986509042143148</v>
-      </c>
-      <c r="I8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9">
-        <v>0.61836412605720692</v>
-      </c>
-      <c r="C9">
-        <v>1.2833239609007259E-5</v>
-      </c>
-      <c r="D9">
-        <v>1.43279947186078E-9</v>
-      </c>
-      <c r="E9">
-        <v>9.3139836105132856E-6</v>
-      </c>
-      <c r="F9">
-        <v>3.5395483123353902E-7</v>
-      </c>
-      <c r="G9">
-        <v>0.3816133713319429</v>
-      </c>
-      <c r="H9">
-        <v>0.61836412605720692</v>
-      </c>
-      <c r="I9" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10">
-        <v>0.67461863819776124</v>
-      </c>
-      <c r="C10">
-        <v>1.070765739450476E-5</v>
-      </c>
-      <c r="D10">
-        <v>6.4447980122478324E-5</v>
-      </c>
-      <c r="E10">
-        <v>1.5435430226466199E-3</v>
-      </c>
-      <c r="F10">
-        <v>1.129653663966973E-3</v>
-      </c>
-      <c r="G10">
-        <v>0.32263300947810808</v>
-      </c>
-      <c r="H10">
-        <v>0.67461863819776124</v>
-      </c>
-      <c r="I10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11">
-        <v>0.59310547204028141</v>
-      </c>
-      <c r="C11">
-        <v>9.0441045868427689E-8</v>
-      </c>
-      <c r="D11">
-        <v>6.1443807867831806E-6</v>
-      </c>
-      <c r="E11">
-        <v>1.6984864756130829E-4</v>
-      </c>
-      <c r="F11">
-        <v>3.4129827679131998E-4</v>
-      </c>
-      <c r="G11">
-        <v>0.40637714621353332</v>
-      </c>
-      <c r="H11">
-        <v>0.59310547204028141</v>
-      </c>
-      <c r="I11" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12">
-        <v>0.67180526370339078</v>
-      </c>
-      <c r="C12">
-        <v>4.2529860053709542E-7</v>
-      </c>
-      <c r="D12">
-        <v>6.4900489368964851E-9</v>
-      </c>
-      <c r="E12">
-        <v>5.5852034419832293E-5</v>
-      </c>
-      <c r="F12">
-        <v>1.4821636319061899E-5</v>
-      </c>
-      <c r="G12">
-        <v>0.3281236308372209</v>
-      </c>
-      <c r="H12">
-        <v>0.67180526370339078</v>
-      </c>
-      <c r="I12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13">
-        <v>0.28315394301584251</v>
-      </c>
-      <c r="C13">
-        <v>1.321603500935837E-5</v>
-      </c>
-      <c r="D13">
-        <v>9.4100572272599924E-6</v>
-      </c>
-      <c r="E13">
-        <v>5.3123937614995664E-4</v>
-      </c>
-      <c r="F13">
-        <v>0.47972576295737768</v>
-      </c>
-      <c r="G13">
-        <v>0.23656642855839319</v>
-      </c>
-      <c r="H13">
-        <v>0.47972576295737768</v>
-      </c>
-      <c r="I13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14">
-        <v>0.72904461093497497</v>
-      </c>
-      <c r="C14">
-        <v>4.1855235465205028E-4</v>
-      </c>
-      <c r="D14">
-        <v>1.9776195674159422E-6</v>
-      </c>
-      <c r="E14">
-        <v>4.8581987100465908E-5</v>
-      </c>
-      <c r="F14">
-        <v>1.3108887048729921E-2</v>
-      </c>
-      <c r="G14">
-        <v>0.25737739005497517</v>
-      </c>
-      <c r="H14">
-        <v>0.72904461093497497</v>
-      </c>
-      <c r="I14" t="s">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B15">
-        <v>0.83532179681551277</v>
-      </c>
-      <c r="C15">
-        <v>2.771067505417387E-5</v>
-      </c>
-      <c r="D15">
-        <v>1.860528096442206E-7</v>
-      </c>
-      <c r="E15">
-        <v>4.0298641427852347E-5</v>
-      </c>
-      <c r="F15">
-        <v>4.7479229213384806E-6</v>
-      </c>
-      <c r="G15">
-        <v>0.16460525989227431</v>
-      </c>
-      <c r="H15">
-        <v>0.83532179681551277</v>
-      </c>
-      <c r="I15" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16">
-        <v>0.54529760465578303</v>
-      </c>
-      <c r="C16">
-        <v>4.8265553023162833E-5</v>
-      </c>
-      <c r="D16">
-        <v>1.8617214815554829E-4</v>
-      </c>
-      <c r="E16">
-        <v>7.7130021586932376E-4</v>
-      </c>
-      <c r="F16">
-        <v>1.788125684848504E-5</v>
-      </c>
-      <c r="G16">
-        <v>0.45367877617032049</v>
-      </c>
-      <c r="H16">
-        <v>0.54529760465578303</v>
-      </c>
-      <c r="I16" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17">
-        <v>0.36559561241577332</v>
-      </c>
-      <c r="C17">
-        <v>3.3227325089374899E-3</v>
-      </c>
-      <c r="D17">
-        <v>7.4093075695210162E-2</v>
-      </c>
-      <c r="E17">
-        <v>6.2561318687197626E-3</v>
-      </c>
-      <c r="F17">
-        <v>1.5410235446974231E-4</v>
-      </c>
-      <c r="G17">
-        <v>0.55057834515688953</v>
-      </c>
-      <c r="H17">
-        <v>0.55057834515688953</v>
-      </c>
-      <c r="I17" t="s">
-        <v>5</v>
-      </c>
-      <c r="J17" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B18">
-        <v>0.50499317065524019</v>
-      </c>
-      <c r="C18">
-        <v>6.8299911222444374E-5</v>
-      </c>
-      <c r="D18">
-        <v>1.85083253173346E-3</v>
-      </c>
-      <c r="E18">
-        <v>8.0768419171518174E-4</v>
-      </c>
-      <c r="F18">
-        <v>4.4610565304888458E-4</v>
-      </c>
-      <c r="G18">
-        <v>0.49183390705703978</v>
-      </c>
-      <c r="H18">
-        <v>0.50499317065524019</v>
-      </c>
-      <c r="I18" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B19">
-        <v>0.58152710776009975</v>
-      </c>
-      <c r="C19">
-        <v>3.1720191540027432E-3</v>
-      </c>
-      <c r="D19">
-        <v>0.19677412894604551</v>
-      </c>
-      <c r="E19">
-        <v>4.6406774332589992E-3</v>
-      </c>
-      <c r="F19">
-        <v>4.9733023537047738E-5</v>
-      </c>
-      <c r="G19">
-        <v>0.21383633368305591</v>
-      </c>
-      <c r="H19">
-        <v>0.58152710776009975</v>
-      </c>
-      <c r="I19" t="s">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B20">
-        <v>0.3477908580454443</v>
-      </c>
-      <c r="C20">
-        <v>3.5168716547516438E-4</v>
-      </c>
-      <c r="D20">
-        <v>5.4962003982457837E-5</v>
-      </c>
-      <c r="E20">
-        <v>3.3823789505798429E-4</v>
-      </c>
-      <c r="F20">
-        <v>1.3187308559477541E-2</v>
-      </c>
-      <c r="G20">
-        <v>0.63827694633056253</v>
-      </c>
-      <c r="H20">
-        <v>0.63827694633056253</v>
-      </c>
-      <c r="I20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J20" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21">
-        <v>0.55720495682682047</v>
-      </c>
-      <c r="C21">
-        <v>2.383467772668843E-4</v>
-      </c>
-      <c r="D21">
-        <v>6.1725396922407319E-4</v>
-      </c>
-      <c r="E21">
-        <v>5.1108286886637473E-4</v>
-      </c>
-      <c r="F21">
-        <v>0.29389988560318758</v>
-      </c>
-      <c r="G21">
-        <v>0.1475284739546347</v>
-      </c>
-      <c r="H21">
-        <v>0.55720495682682047</v>
-      </c>
-      <c r="I21" t="s">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B22">
-        <v>0.80045373845278855</v>
-      </c>
-      <c r="C22">
-        <v>1.1171577191273651E-6</v>
-      </c>
-      <c r="D22">
-        <v>5.3257826086235674E-6</v>
-      </c>
-      <c r="E22">
-        <v>1.7920049714070471E-4</v>
-      </c>
-      <c r="F22">
-        <v>1.226658673256531E-2</v>
-      </c>
-      <c r="G22">
-        <v>0.1870940313771777</v>
-      </c>
-      <c r="H22">
-        <v>0.80045373845278855</v>
-      </c>
-      <c r="I22" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B23">
-        <v>0.59297012281514916</v>
-      </c>
-      <c r="C23">
-        <v>1.4595449710584949E-4</v>
-      </c>
-      <c r="D23">
-        <v>0.1291327397852223</v>
-      </c>
-      <c r="E23">
-        <v>8.0884954008217241E-3</v>
-      </c>
-      <c r="F23">
-        <v>2.989132753724155E-3</v>
-      </c>
-      <c r="G23">
-        <v>0.26667355474797672</v>
-      </c>
-      <c r="H23">
-        <v>0.59297012281514916</v>
-      </c>
-      <c r="I23" t="s">
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B24">
-        <v>0.57945253748866643</v>
-      </c>
-      <c r="C24">
-        <v>3.1448842333005111E-4</v>
-      </c>
-      <c r="D24">
-        <v>1.127062697055716E-4</v>
-      </c>
-      <c r="E24">
-        <v>2.1080369066949389E-4</v>
-      </c>
-      <c r="F24">
-        <v>5.5488070968100368E-3</v>
-      </c>
-      <c r="G24">
-        <v>0.41436065703081848</v>
-      </c>
-      <c r="H24">
-        <v>0.57945253748866643</v>
-      </c>
-      <c r="I24" t="s">
-        <v>0</v>
-      </c>
-      <c r="J24" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B25">
-        <v>0.15350851579812111</v>
-      </c>
-      <c r="C25">
-        <v>1.226996494366378E-6</v>
-      </c>
-      <c r="D25">
-        <v>3.0296096395602149E-5</v>
-      </c>
-      <c r="E25">
-        <v>3.0872610549692619E-4</v>
-      </c>
-      <c r="F25">
-        <v>0.1068015002849167</v>
-      </c>
-      <c r="G25">
-        <v>0.73934973471857524</v>
-      </c>
-      <c r="H25">
-        <v>0.73934973471857524</v>
-      </c>
-      <c r="I25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J25" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B26">
-        <v>0.44011129040500158</v>
-      </c>
-      <c r="C26">
-        <v>6.6036093996594224E-4</v>
-      </c>
-      <c r="D26">
-        <v>2.1048801993760351E-2</v>
-      </c>
-      <c r="E26">
-        <v>8.2214609446061278E-4</v>
-      </c>
-      <c r="F26">
-        <v>2.728135626163247E-6</v>
-      </c>
-      <c r="G26">
-        <v>0.53735467243118529</v>
-      </c>
-      <c r="H26">
-        <v>0.53735467243118529</v>
-      </c>
-      <c r="I26" t="s">
-        <v>5</v>
-      </c>
-      <c r="J26" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B27">
-        <v>0.77098359980791509</v>
-      </c>
-      <c r="C27">
-        <v>3.9956364069023492E-5</v>
-      </c>
-      <c r="D27">
-        <v>6.5655279092271171E-8</v>
-      </c>
-      <c r="E27">
-        <v>2.5168604183040268E-4</v>
-      </c>
-      <c r="F27">
-        <v>4.8978401821334118E-5</v>
-      </c>
-      <c r="G27">
-        <v>0.22867571372908499</v>
-      </c>
-      <c r="H27">
-        <v>0.77098359980791509</v>
-      </c>
-      <c r="I27" t="s">
-        <v>0</v>
-      </c>
-      <c r="J27" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B28">
-        <v>0.8260576602052262</v>
-      </c>
-      <c r="C28">
-        <v>5.1443094474889997E-5</v>
-      </c>
-      <c r="D28">
-        <v>1.217570639969568E-4</v>
-      </c>
-      <c r="E28">
-        <v>7.2891948072552625E-5</v>
-      </c>
-      <c r="F28">
-        <v>6.6079247982626802E-3</v>
-      </c>
-      <c r="G28">
-        <v>0.1670883228899667</v>
-      </c>
-      <c r="H28">
-        <v>0.8260576602052262</v>
-      </c>
-      <c r="I28" t="s">
-        <v>0</v>
-      </c>
-      <c r="J28" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B29">
-        <v>0.81070142317998728</v>
-      </c>
-      <c r="C29">
-        <v>1.3558250337925289E-4</v>
-      </c>
-      <c r="D29">
-        <v>1.3575181306151401E-3</v>
-      </c>
-      <c r="E29">
-        <v>5.1242426316290134E-4</v>
-      </c>
-      <c r="F29">
-        <v>1.5050260687538011E-4</v>
-      </c>
-      <c r="G29">
-        <v>0.18714254931598001</v>
-      </c>
-      <c r="H29">
-        <v>0.81070142317998728</v>
-      </c>
-      <c r="I29" t="s">
-        <v>0</v>
-      </c>
-      <c r="J29" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B30">
-        <v>0.29445723391376788</v>
-      </c>
-      <c r="C30">
-        <v>6.4490839084839404E-3</v>
-      </c>
-      <c r="D30">
-        <v>4.9007350266938048E-6</v>
-      </c>
-      <c r="E30">
-        <v>6.5547918229123692E-3</v>
-      </c>
-      <c r="F30">
-        <v>0.20987841999268761</v>
-      </c>
-      <c r="G30">
-        <v>0.48265556962712147</v>
-      </c>
-      <c r="H30">
-        <v>0.48265556962712147</v>
-      </c>
-      <c r="I30" t="s">
-        <v>5</v>
-      </c>
-      <c r="J30" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B31">
-        <v>1.2121312646791499E-2</v>
-      </c>
-      <c r="C31">
-        <v>2.6491047920619467E-4</v>
-      </c>
-      <c r="D31">
-        <v>0.97065545339003312</v>
-      </c>
-      <c r="E31">
-        <v>5.7511427090164313E-5</v>
-      </c>
-      <c r="F31">
-        <v>6.8171902344283191E-5</v>
-      </c>
-      <c r="G31">
-        <v>1.6832640154534721E-2</v>
-      </c>
-      <c r="H31">
-        <v>0.97065545339003312</v>
-      </c>
-      <c r="I31" t="s">
-        <v>2</v>
-      </c>
-      <c r="J31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B32">
-        <v>0.22656978044018511</v>
-      </c>
-      <c r="C32">
-        <v>3.702642955274395E-6</v>
-      </c>
-      <c r="D32">
-        <v>6.0084820324630167E-2</v>
-      </c>
-      <c r="E32">
-        <v>2.258867703772109E-4</v>
-      </c>
-      <c r="F32">
-        <v>4.5131180270008937E-3</v>
-      </c>
-      <c r="G32">
-        <v>0.70860269179485136</v>
-      </c>
-      <c r="H32">
-        <v>0.70860269179485136</v>
-      </c>
-      <c r="I32" t="s">
-        <v>5</v>
-      </c>
-      <c r="J32" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B33">
-        <v>0.39832937722265571</v>
-      </c>
-      <c r="C33">
-        <v>3.9745749864807536E-6</v>
-      </c>
-      <c r="D33">
-        <v>5.1040354796053018E-6</v>
-      </c>
-      <c r="E33">
-        <v>1.1594048314780331E-3</v>
-      </c>
-      <c r="F33">
-        <v>1.7911091557380049E-6</v>
-      </c>
-      <c r="G33">
-        <v>0.60050034822624432</v>
-      </c>
-      <c r="H33">
-        <v>0.60050034822624432</v>
-      </c>
-      <c r="I33" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B34">
-        <v>0.46558300552967219</v>
-      </c>
-      <c r="C34">
-        <v>1.139090495998097E-4</v>
-      </c>
-      <c r="D34">
-        <v>9.5602360153714868E-3</v>
-      </c>
-      <c r="E34">
-        <v>2.6733986983095462E-4</v>
-      </c>
-      <c r="F34">
-        <v>7.7287863092794765E-5</v>
-      </c>
-      <c r="G34">
-        <v>0.52439822167243266</v>
-      </c>
-      <c r="H34">
-        <v>0.52439822167243266</v>
-      </c>
-      <c r="I34" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" t="s">
-        <v>703</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H132"/>

</xml_diff>